<commit_message>
The model was ran with data sice 2020-2024, the prob_win was sort according the highest probabily. the rule was 1.5 in order until the total_money runs out
</commit_message>
<xml_diff>
--- a/data/output/results/winner_metrics_class.xlsx
+++ b/data/output/results/winner_metrics_class.xlsx
@@ -477,27 +477,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6529282804081515</v>
+        <v>0.7164494012499029</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6529195011337868</v>
+        <v>0.7164493408842145</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6529096085077205</v>
+        <v>0.7164493539284298</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">[1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, </t>
+          <t>[1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[[0.4953556090185732, 0.5046443909814269], [0.46554874758537795, 0.5344512524146221], [0.3636300576950427, 0.6363699423049574], [0.5550639401234021, 0.44493605987659784], [0.6119115844792593, 0.3880884155207407], [0.49849584759923093, 0.5015041524007691], [0.4595856877084284, 0.5404143122915717], [0.5036732095733436, 0.4963267904266563], [0.3581770874579921, 0.6418229125420079], [0.5050022279706436, 0.4949977720293563], [0.5192070915157516, 0.4807929084842484], [0.45738248202244935, 0.5426175179775508], [0.47964628495669087, 0.5203537150433092], [0.5814806913857861, 0.4185193086142139], [0.5227514642010519, 0.4772485357989481], [0.49793295439331997, 0.50206704560668], [0.5492019138388365, 0.4507980861611634], [0.5815494580738102, 0.4184505419261898], [0.3517011246945466, 0.6482988753054533], [0.39866165203982407, 0.6013383479601759], [0.9107997415044152, 0.0892002584955848], [0.9795446813589241, 0.02045531864107574], [0.5377421237741593, 0.4622578762258407], [0.26616245013730133, 0.7338375498626986], [0.36883484984725845, 0.6311651501527417], [0.558532727410976, 0.4414672725890239], [0.5751969341641752, 0.42480306583582483], [0.5733403837641391, 0.4266596162358608], [0.5184546394924605, 0.4815453605075395], [0.9202225342804722, 0.07977746571952786], [0.5364609854276332, 0.46353901457236674], [0.40021127843605797, 0.599788721563942], [0.5600791012257876, 0.43992089877421225], [0.5400859400425584, 0.4599140599574415], [0.5210234356913609, 0.4789765643086391], [0.4836438047693159, 0.5163561952306841], [0.4844494195226436, 0.5155505804773564], [0.5877421682143288, 0.41225783178567116], [0.4771552411068291, 0.522844758893171], [0.49091019829694, 0.5090898017030601], [0.5411789923903662, 0.4588210076096339], [0.3730818013781169, 0.6269181986218831], [0.5138190141147945, 0.4861809858852056], [0.583432157785343, 0.4165678422146569], [0.4061827309562728, 0.5938172690437272], [0.10266350747149414, 0.8973364925285058], [0.5812379974773801, 0.4187620025226199], [0.6124678820974164, 0.38753211790258346], [0.913248093341828, 0.08675190665817188], [0.5628947033311351, 0.43710529666886494], [0.5518548510000089, 0.44814514899999125], [0.4569901357889148, 0.5430098642110852], [0.34003972614426514, 0.6599602738557349], [0.46869518777360775, 0.5313048122263921], [0.5307425399467841, 0.46925746005321595], [0.28862543658611944, 0.7113745634138806], [0.5193787256760366, 0.48062127432396345], [0.17915595205786974, 0.8208440479421302], [0.988018454783411, 0.011981545216588934], [0.44656514599628794, 0.5534348540037121], [0.4810612489975649, 0.5189387510024351], [0.3883877167817002, 0.6116122832182999], [0.7005362637651803, 0.2994637362348197], [0.39437610361601794, 0.6056238963839821], [0.5447461946266029, 0.4552538053733972], [0.4928489092696829, 0.5071510907303171], [0.5305648375772672, 0.46943516242273275], [0.48717412906094426, 0.5128258709390557], [0.9661135264605005, 0.03388647353949941], [0.5145456250431241, 0.4854543749568759], [0.4144922649619591, 0.585507735038041], [0.23486754506408372, 0.7651324549359164], [0.5101003888991129, 0.48989961110088703], [0.228249710372398, 0.7717502896276021], [0.5375371470195307, 0.4624628529804692], [0.6169971467917208, 0.3830028532082792], [0.3530417725684919, 0.646958227431508], [0.5267883836517604, 0.47321161634823955], [0.46854356325333807, 0.531456436746662], [0.04758446228363216, 0.9524155377163679], [0.029067345131331173, 0.9709326548686689], [0.5101700386818128, 0.4898299613181873], [0.5304311658711336, 0.4695688341288664], [0.8471805460673922, 0.15281945393260782], [0.9481025013208438, 0.05189749867915622], [0.9359621434414369, 0.06403785655856295], [0.5488692083692234, 0.4511307916307766], [0.6557197743749882, 0.34428022562501187], [0.5279568349347836, 0.47204316506521643], [0.4492740230071098, 0.5507259769928902], [0.5918657280813059, 0.40813427191869417], [0.4920365509227769, 0.5079634490772231], [0.49389131019632904, 0.506108689803671], [0.51319993559908, 0.48680006440092005], [0.4095205843916193, 0.5904794156083807], [0.4521319642177186, 0.5478680357822815], [0.3304328830012934, 0.6695671169987065], [0.5202687440913314, 0.47973125590866855], [0.4244875443027968, 0.5755124556972032], [0.6447145566415973, 0.35528544335840273], [0.23781980052663443, 0.7621801994733656], [0.6391673416420743, 0.36083265835792566], [0.16321671089238754, 0.8367832891076125], [0.7957346997748087, 0.2042653002251913], [0.3173488566932556, 0.6826511433067444], [0.08327079568720312, 0.9167292043127969], [0.305646619967041, 0.694353380032959], [0.5714194213402011, 0.428580578659799], [0.4011715758847125, 0.5988284241152876], [0.7193115575265732, 0.28068844247342684], [0.1610927045851968, 0.8389072954148031], [0.9832034153334694, 0.016796584666530587], [0.37617867556139845, 0.6238213244386016], [0.4904250696442238, 0.5095749303557762], [0.2793215407140368, 0.7206784592859632], [0.6048740238915855, 0.39512597610841443], [0.33310661553450205, 0.666893384465498], [0.2559683089801162, 0.7440316910198838], [0.6842973728715017, 0.3157026271284983], [0.7464837685047293, 0.2535162314952706], [0.5935473565426649, 0.40645264345733506], [0.3523102121934801, 0.64768978780652], [0.5192406143377059, 0.48075938566229415], [0.5103398981560667, 0.48966010184393327], [0.47870664392392476, 0.5212933560760753], [0.38823938309753336, 0.6117606169024666], [0.4171566034676593, 0.5828433965323407], [0.4190191688256793, 0.5809808311743208], [0.6497119704968927, 0.35028802950310733], [0.24295572040456853, 0.7570442795954315], [0.6074634467008099, 0.3925365532991901], [0.5898460487771757, 0.4101539512228243], [0.521684191423845, 0.47831580857615497], [0.3359644638931025, 0.6640355361068975], [0.5083352328266095, 0.4916647671733905], [0.5136252034415169, 0.48637479655848304], [0.4474150755120904, 0.5525849244879096], [0.5333149523994262, 0.4666850476005738], [0.30440689057630743, 0.6955931094236926], [0.5607184223299743, 0.4392815776700258], [0.5264061440370021, 0.4735938559629978], [0.39820918544078227, 0.6017908145592177], [0.2254813213322074, 0.7745186786677926], [0.562660120531741, 0.4373398794682589], [0.5849785442167582, 0.4150214557832418], [0.5494016469915085, 0.4505983530084915], [0.2391618229168957, 0.7608381770831043], [0.975837314706233, 0.02416268529376689], [0.4980961010909661, 0.5019038989090339], [0.36599826666613533, 0.6340017333338648], [0.4996106451243046, 0.5003893548756955], [0.5049372492337098, 0.49506275076629025], [0.4541772498975248, 0.5458227501024752], [0.47590171414953225, 0.5240982858504677], [0.67304241990729, 0.3269575800927101], [0.5597232626560075, 0.44027673734399264], [0.417824405378058, 0.5821755946219419], [0.5154130396334832, 0.4845869603665168], [0.47258473728349476, 0.5274152627165052], [0.4000946876805027, 0.5999053123194973], [0.5216865583727957, 0.4783134416272044], [0.5379942244998968, 0.46200577550010324], [0.49503040312052227, 0.5049695968794777], [0.5333557836339685, 0.4666442163660315], [0.369142114094364, 0.6308578859056361], [0.042133409943471443, 0.9578665900565285], [0.48734010303785213, 0.5126598969621479], [0.685067558970065, 0.31493244102993495], [0.5526195950315197, 0.4473804049684802], [0.15885782882037017, 0.8411421711796299], [0.27798545915222467, 0.7220145408477754], [0.7080067514405229, 0.29199324855947706], [0.4034273161247111, 0.596572683875289], [0.5034631624131903, 0.4965368375868097], [0.25405832058987027, 0.7459416794101297], [0.8087511490301832, 0.19124885096981675], [0.5466196695896679, 0.4533803304103321], [0.2663488896502753, 0.7336511103497246], [0.3473758394956566, 0.6526241605043435], [0.7675390593655761, 0.232460940634424], [0.282421719212903, 0.7175782807870971], [0.6499947695366955, 0.35000523046330445], [0.4260477118962571, 0.5739522881037429], [0.592087315127432, 0.40791268487256804], [0.32098770091091694, 0.6790122990890831], [0.5748381133001881, 0.42516188669981203], [0.20099641293775197, 0.799003587062248], [0.3400844294803068, 0.6599155705196932], [0.46427122690387984, 0.5357287730961201], [0.5924821038192473, 0.40751789618075285], [0.6087938879457016, 0.39120611205429845], [0.30053611368948985, 0.6994638863105102], [0.3338870503450246, 0.6661129496549754], [0.585061183778713, 0.41493881622128703], [0.52830466972486, 0.47169533027514], [0.44757916565007827, 0.5524208343499218], [0.3611579502261029, 0.6388420497738971], [0.6418734382990483, 0.35812656170095175], [0.7054212298254171, 0.2945787701745829], [0.5892389603042711, 0.41076103969572886], [0.4078616681965892, 0.5921383318034108], [0.6181229626274592, 0.38187703737254075], [0.267887095450191, 0.7321129045498089], [0.5072530401434588, 0.49274695985654116], [0.015167458999730479, 0.9848325410002694], [0.6044045095775669, 0.39559549042243314], [0.7079327854336502, 0.29206721456634965], [0.0033421391781755646, 0.9966578608218244], [0.8727540882448008, 0.12724591175519923], [0.3579108240490282, 0.6420891759509718], [0.36291599602178026, 0.6370840039782197], [0.6447590441933494, 0.3552409558066506], [0.4293586033208198, 0.5706413966791801], [0.5685495440258608, 0.43145045597413934], [0.8845515534744096, 0.11544844652559029], [0.49681733067208517, 0.5031826693279148], [0.4155267144798894, 0.5844732855201106], [0.5669940196787152, 0.4330059803212848], [0.5275963193813108, 0.4724036806186891], [0.5588233797830033, 0.4411766202169966], [0.6940286304488409, 0.30597136955115917], [0.5184156962009088, 0.4815843037990913], [0.4438582465160153, 0.5561417534839848], [0.5106490295834389, 0.48935097041656106], [0.5372087746225533, 0.46279122537744666], [0.4108855889096014, 0.5891144110903985], [0.873281183033902, 0.12671881696609805], [0.43339836746306765, 0.5666016325369324], [0.6203566167666142, 0.37964338323338576], [0.4541682427200274, 0.5458317572799726], [0.4801866659881726, 0.5198133340118274], [0.5691130892825279, 0.4308869107174721], [0.4762542823226129, 0.5237457176773871], [0.6329887274320527, 0.3670112725679474], [0.5227221372082426, 0.47727786279175743], [0.9305850908432365, 0.06941490915676357], [0.49849786939775936, 0.5015021306022407], [0.3499238391725678, 0.6500761608274321], [0.4571815718441305, 0.5428184281558696], [0.6689537005483888, 0.33104629945161124], [0.6362017572579864, 0.36379824274201356], [0.6152908400531181, 0.38470915994688193], [0.6003392426515265, 0.3996607573484736], [0.623666820141957, 0.3763331798580431], [0.4832388139211454, 0.5167611860788546], [0.5729921792336291, 0.42700782076637095], [0.5357338026934528, 0.4642661973065471], [0.029433234507160802, 0.9705667654928392], [0.841755048119207, 0.15824495188079307], [0.5087491576797064, 0.4912508423202937], [0.6417111628740902, 0.3582888371259097], [0.559597858906851, 0.44040214109314907], [0.7664211072969627, 0.2335788927030373], [0.5275038462408221, 0.47249615375917786], [0.5420613960143899, 0.45793860398561015], [0.41625538646222304, 0.583744613537777], [0.4918324547956858, 0.5081675452043142], [0.19423450943499898, 0.805765490565001], [0.5352452814091533, 0.4647547185908468], [0.27153590138961614, 0.7284640986103837], [0.3668585401735509, 0.6331414598264491], [0.4826762465456271, 0.517323753454373], [0.3118343177909884, 0.6881656822090115], [0.46964903682888814, 0.5303509631711117], [0.49610867468944475, 0.5038913253105552], [0.5027444030899116, 0.49725559691008836], [0.32552782126477753, 0.6744721787352226], [0.38319662580480013, 0.6168033741951998], [0.02327338722090485, 0.9767266127790951], [0.8644229985531946, 0.13557700144680537], [0.4097665784464141, 0.5902334215535858], [0.5530079937896227, 0.44699200621037727], [0.6322842944347149, 0.3677157055652851], [0.24829357622384027, 0.7517064237761597], [0.5400950377373325, 0.45990496226266747], [0.046239352407740936, 0.9537606475922591], [0.34953218408220843, 0.6504678159177916], [0.7649835314029215, 0.23501646859707842], [0.3534379735486405, 0.6465620264513594], [0.6586403618490696, 0.34135963815093034], [0.6163020271561094, 0.38369797284389073], [0.56909893134446, 0.43090106865554], [0.36459490200385064, 0.6354050979961494], [0.5575849869895844, 0.44241501301041564], [0.5050572349824212, 0.49494276501757883], [0.5324599242040812, 0.46754007579591883], [0.4699287956401997, 0.5300712043598003], [0.5640607007851874, 0.43593929921481256], [0.5269821631811227, 0.47301783681887727], [0.3816505041307457, 0.6183494958692543], [0.3445977857369109, 0.6554022142630892], [0.4359894156956821, 0.5640105843043179], [0.5035285687205633, 0.4964714312794367], [0.49239198383631955, 0.5076080161636805], [0.6520090743318748, 0.3479909256681252], [0.49160112362685204, 0.508398876373148], [0.5459500336073385, 0.45404996639266154], [0.4316691288189339, 0.5683308711810661], [0.45301731887454466, 0.5469826811254553], [0.5808884881105264, 0.4191115118894736], [0.5114780476694363, 0.48852195233056367], [0.6509052546214729, 0.349094745378527], [0.6013657193235982, 0.39863428067640194], [0.5268896936966085, 0.4731103063033914], [0.5915073999196714, 0.40849260008032867], [0.6387085160694389, 0.36129148393056104], [0.4744589457353385, 0.5255410542646616], [0.5207798056896824, 0.47922019431031754], [0.9101548573345428, 0.0898451426654571], [0.792539939215559, 0.20746006078444107], [0.38185048303611474, 0.6181495169638853], [0.5289827873331646, 0.4710172126668355], [0.38516509222752937, 0.6148349077724706], [0.45659091338937363, 0.5434090866106264], [0.49221030037035335, 0.5077896996296467], [0.7315819474627204, 0.26841805253727963], [0.5342357865769002, 0.4657642134230999], [0.5359223220304301, 0.4640776779695699], [0.45899070819039667, 0.5410092918096032], [0.6753089196451239, 0.3246910803548762], [0.9020089506980609, 0.09799104930193912], [0.5332581649079368, 0.46674183509206335], [0.3326623346065127, 0.6673376653934874], [0.4067862005343148, 0.5932137994656852], [0.5163953076073531, 0.48360469239264686], [0.28236307741999417, 0.7176369225800058], [0.5289415223985556, 0.47105847760144437], [0.5681529275067453, 0.43184707249325477], [0.5540337148731516, 0.4459662851268484], [0.4458634157276272, 0.5541365842723728], [0.3674124380407435, 0.6325875619592565], [0.3197182480779247, 0.6802817519220754], [0.4949622826312347, 0.5050377173687652], [0.36559663172416007, 0.63440336827584], [0.749063738530833, 0.25093626146916703], [0.5319182398938733, 0.46808176010612673], [0.03920704184863056, 0.9607929581513693], [0.4821261242415086, 0.5178738757584914], [0.47767721886716974, 0.5223227811328304], [0.673248616163277, 0.3267513838367229], [0.020771534235605783, 0.9792284657643943], [0.6952963922544909, 0.3047036077455092], [0.23917290805955502, 0.7608270919404451], [0.13647007196574867, 0.8635299280342513], [0.23373555550076303, 0.766264444499237], [0.3639291357963673, 0.6360708642036327], [0.3874219214479543, 0.6125780785520458], [0.6418146473329734, 0.3581853526670265], [0.4695230370684119, 0.5304769629315881], [0.9211013166360021, 0.07889868336399793], [0.33265011950280193, 0.6673498804971981], [0.12032603227759392, 0.8796739677224061], [0.376157143790357, 0.6238428562096431], [0.5695499070453081, 0.43045009295469194], [0.17001004765561467, 0.8299899523443852], [0.9041859994679523, 0.0958140005320476], [0.9837143342759788, 0.01628566572402116], [0.46659240211767766, 0.5334075978823224], [0.45462533011153067, 0.5453746698884694], [0.13445633531020434, 0.8655436646897956], [0.3278182244987309, 0.6721817755012692], [0.3976117274493543, 0.6023882725506458], [0.4045560212095207, 0.5954439787904792], [0.45150868700286245, 0.5484913129971376], [0.38940767844886237, 0.6105923215511376], [0.4449155518683503, 0.5550844481316497], [0.453590685889765, 0.546409314110235], [0.5281191375958649, 0.47188086240413507], [0.49228099996799046, 0.5077190000320095], [0.43644067598239084, 0.5635593240176092], [0.3331487080759829, 0.666851291924017], [0.52625044664075, 0.4737495533592499], [0.6099517182835954, 0.39004828171640465], [0.35947681560734646, 0.6405231843926537], [0.5142845048087019, 0.48571549519129814], [0.47627180213443243, 0.5237281978655676], [0.5399181618610438, 0.4600818381389562], [0.6463970078782347, 0.35360299212176527], [0.5277782692005946, 0.4722217307994054], [0.46820441699986287, 0.5317955830001372], [0.8864652221015186, 0.11353477789848145], [0.6219336341432455, 0.3780663658567544], [0.5539086719684435, 0.44609132803155643], [0.2492879476819521, 0.7507120523180479], [0.6252637804546244, 0.37473621954537556], [0.48916151527610696, 0.5108384847238929], [0.48955987854787486, 0.5104401214521251], [0.48368562829988865, 0.5163143717001113], [0.055152625144804575, 0.9448473748551953], [0.5829384602572871, 0.4170615397427129], [0.4137297127263678, 0.5862702872736323], [0.2057822399818391, 0.7942177600181609], [0.476138988889033, 0.523861011110967], [0.557202848505857, 0.4427971514941429], [0.2926451962971303, 0.7073548037028696], [0.36838088431467736, 0.6316191156853227], [0.4861309210538139, 0.5138690789461862], [0.7119939260486734, 0.28800607395132666], [0.4737150200137313, 0.5262849799862688], [0.3555663889232669, 0.644433611076733], [0.5439516504972794, 0.45604834950272055], [0.47265293943464537, 0.5273470605653547], [0.37572460996833695, 0.6242753900316631], [0.5046684969963943, 0.49533150300360573], [0.452098733169586, 0.547901266830414], [0.5036034924444746, 0.4963965075555254], [0.5063840450653666, 0.4936159549346334], [0.9377640040166171, 0.06223599598338286], [0.5678764930757102, 0.43212350692428975], [0.3466696446436408, 0.6533303553563593], [0.4749731097659531, 0.525026890234047], [0.8166896031761466, 0.18331039682385336], [0.30105364425810965, 0.6989463557418902], [0.32881339157780654, 0.6711866084221935], [0.5404656140867926, 0.4595343859132074], [0.6192699209431674, 0.38073007905683265], [0.41737339160015163, 0.5826266083998484], [0.22324687263819962, 0.7767531273618002], [0.3586673477121489, 0.6413326522878511], [0.5259285370178127, 0.47407146298218716], [0.4984925472957827, 0.5015074527042174], [0.524266598825665, 0.475733401174335], [0.5183465402948195, 0.48165345970518053], [0.5670895019381567, 0.43291049806184334], [0.4794608786925416, 0.5205391213074584], [0.5415658365828635, 0.4584341634171365], [0.16497235971949667, 0.8350276402805034], [0.5669226261922561, 0.43307737380774386], [0.5823577560443105, 0.41764224395568955], [0.32059389580232817, 0.6794061041976719], [0.713260332840995, 0.286739667159005], [0.315324999924381, 0.6846750000756191], [0.44672207770343264, 0.5532779222965674], [0.3825744921527564, 0.6174255078472436], [0.4011812832910562, 0.5988187167089438], [0.41333424917089034, 0.5866657508291097], [0.6506683457187952, 0.34933165428120483], [0.9389076507092278, 0.061092349290772244], [0.5048233317556464, 0.4951766682443536], [0.7361006022291424, 0.2638993977708577], [0.4892087716617251, 0.5107912283382748], [0.3994223832354252, 0.6005776167645748], [0.287335328352591, 0.712664671647409], [0.5956921636764821, 0.4043078363235179], [0.5581828011651412, 0.44181719883485887], [0.9154975754641074, 0.08450242453589266], [0.4701536175593408, 0.5298463824406592], [0.10013622252371897, 0.8998637774762811], [0.5412548738524947, 0.4587451261475054], [0.5325248204365322, 0.46747517956346785], [0.4818512808344691, 0.5181487191655308], [0.6667642935062883, 0.33323570649371165], [0.5993937684524091, 0.40060623154759095], [0.16062790754520528, 0.8393720924547948], [0.5036382942271018, 0.49636170577289823], [0.3841607181690003, 0.6158392818309997], [0.5250136666251872, 0.4749863333748127], [0.475463401607546, 0.524536598392454], [0.5206112610647345, 0.47938873893526546], [0.2781879191410625, 0.7218120808589374], [0.5456964671318371, 0.45430353286816294], [0.5047546558867022, 0.49524534411329785], [0.5159997032589, 0.4840002967411001], [0.2249589256935436, 0.7750410743064564], [0.49814044302878807, 0.501859556971212], [0.6963078742664829, 0.30369212573351717], [0.4209322212014371, 0.579067778798563], [0.7230999354878478, 0.27690006451215227], [0.9061164633742956, 0.09388353662570441], [0.218370446290556, 0.781629553709444], [0.4756784462919929, 0.5243215537080071], [0.5892953476353167, 0.41070465236468334], [0.38617933128467347, 0.6138206687153266], [0.5135427793847545, 0.4864572206152455], [0.46989638007211165, 0.5301036199278882], [0.48970378507877316, 0.5102962149212268], [0.46970414595579957, 0.5302958540442004], [0.5077424954298404, 0.49225750457015965], [0.832790978064345, 0.16720902193565504], [0.5599367402772126, 0.44006325972278737], [0.5320909484191454, 0.4679090515808546], [0.4082216148084976, 0.5917783851915025], [0.4692975810983228, 0.5307024189016771], [0.009441257391796362, 0.9905587426082036], [0.5391015888441524, 0.4608984111558476], [0.5052551427980772, 0.4947448572019229], [0.46039101414593087, 0.5396089858540691], [0.4799191868724188, 0.5200808131275811], [0.33723244330605395, 0.662767556693946], [0.017444848252601026, 0.9825551517473989], [0.4496963132930191, 0.5503036867069808], [0.5854053079119799, 0.4145946920880202], [0.6225926665616832, 0.37740733343831684], [0.6410112906935747, 0.35898870930642524], [0.6454764682853728, 0.35452353171462714], [0.2590468066048312, 0.7409531933951689], [0.9561057975209937, 0.04389420247900633], [0.4365845947644764, 0.5634154052355235], [0.9669296513350789, 0.03307034866492096], [0.5816535327733346, 0.4183464672266654], [0.4143470923748181, 0.5856529076251819], [0.4970094746076802, 0.5029905253923198], [0.4885797379553679, 0.5114202620446321], [0.39015395339418923, 0.6098460466058108], [0.5381882465378321, 0.46181175346216785], [0.46299260762440264, 0.5370073923755974], [0.5893727191843455, 0.41062728081565447], [0.44999618036024436, 0.5500038196397556], [0.4967318164604802, 0.5032681835395199], [0.7716290739568926, 0.22837092604310735], [0.3207058619906921, 0.6792941380093079], [0.631871807185164, 0.3681281928148359], [0.07290890229079361, 0.9270910977092064], [0.6951478275433824, 0.3048521724566176], [0.43861305739902867, 0.5613869426009712], [0.5512746772694586, 0.44872532273054144], [0.6022908030035916, 0.3977091969964084], [0.5240717185015952, 0.4759282814984048], [0.06482908911037269, 0.9351709108896272], [0.48560627549825996, 0.51439372450174], [0.5190898000012725, 0.48091019999872753], [0.31893967265132916, 0.6810603273486708], [0.18235695593554105, 0.8176430440644589], [0.116991184851261, 0.8830088151487389], [0.46949746878468723, 0.5305025312153128], [0.4153905854797168, 0.5846094145202831], [0.5505879999443749, 0.4494120000556251], [0.40304851489811166, 0.5969514851018883], [0.5277601326953666, 0.4722398673046334], [0.570083309468345, 0.42991669053165504], [0.40566734929798387, 0.5943326507020161], [0.7195591775814348, 0.28044082241856516], [0.3628953729848907, 0.6371046270151093], [0.5218231241349905, 0.4781768758650094], [0.2903633721003659, 0.7096366278996341], [0.43030926874048986, 0.5696907312595102], [0.5188287416285089, 0.4811712583714911], [0.48742417904194635, 0.5125758209580535], [0.47494621007203164, 0.5250537899279684], [0.10717519677361323, 0.8928248032263867], [0.523655340934359, 0.47634465906564105], [0.6738348279784248, 0.32616517202157536], [0.7042792486549053, 0.2957207513450947], [0.6581214875829962, 0.3418785124170038], [0.7435085594681597, 0.2564914405318403], [0.5572573218417485, 0.4427426781582516], [0.20821676711731033, 0.7917832328826896], [0.35985413477911693, 0.6401458652208831], [0.6713077494927329, 0.3286922505072671], [0.4158260118842843, 0.5841739881157156], [0.4353251703744175, 0.5646748296255825], [0.2641221930811205, 0.7358778069188796], [0.4817608140315232, 0.5182391859684768], [0.3991803509533372, 0.6008196490466627], [0.1832399734813295, 0.8167600265186704], [0.47607542633838557, 0.5239245736616145], [0.8478542037447407, 0.1521457962552592], [0.514521248426752, 0.485478751573248], [0.5866107347068655, 0.4133892652931346], [0.6846816758606666, 0.3153183241393335], [0.17010770163493008, 0.8298922983650698], [0.44047800278800087, 0.5595219972119991], [0.5224226633074801, 0.4775773366925198], [0.5184576917475222, 0.48154230825247785], [0.3728402347738475, 0.6271597652261526], [0.419760071268873, 0.5802399287311271], [0.40112159535926545, 0.5988784046407345], [0.31010866046298824, 0.6898913395370119], [0.5464749373876433, 0.45352506261235676], [0.4533057867414823, 0.5466942132585176], [0.9467000427479103, 0.05329995725208976], [0.38569839214216084, 0.6143016078578393], [0.692392235924731, 0.3076077640752689], [0.6578688104415277, 0.3421311895584724], [0.5618827667548182, 0.43811723324518187], [0.9466404526178416, 0.053359547382158354], [0.08624114371606117, 0.9137588562839388], [0.5749280996605117, 0.4250719003394883], [0.8266386462436183, 0.17336135375638173], [0.4134269429662093, 0.5865730570337906], [0.5759266597259817, 0.42407334027401833], [0.465650000323019, 0.534349999676981], [0.41095983672354447, 0.5890401632764555], [0.6206241979186741, 0.37937580208132593], [0.5291295369852627, 0.47087046301473723], [0.5308113257649894, 0.46918867423501054], [0.43524225668560096, 0.564757743314399], [0.39129604683477487, 0.6087039531652251], [0.6033405876549967, 0.3966594123450034], [0.6782154074097894, 0.32178459259021064], [0.29933056308779515, 0.7006694369122048], [0.48912027084026116, 0.5108797291597388], [0.43036336668016256, 0.5696366333198375], [0.06435841425861952, 0.9356415857413806], [0.32087995985053813, 0.6791200401494618], [0.536803125350031, 0.463196874649969], [0.5035212955082772, 0.49647870449172277], [0.48726735189658815, 0.5127326481034119], [0.5399418876093839, 0.46005811239061617], [0.4845490207072139, 0.515450979292786], [0.36233144437266623, 0.6376685556273338], [0.2651155386344813, 0.7348844613655188], [0.5479469804709218, 0.4520530195290781], [0.3595316767005813, 0.6404683232994188], [0.8229001619178135, 0.17709983808218646], [0.49136796556363294, 0.5086320344363671], [0.6669709209512124, 0.3330290790487876], [0.44121224218637806, 0.5587877578136219], [0.9814586564589027, 0.018541343541097353], [0.5824593033952644, 0.4175406966047356], [0.49242853599825775, 0.5075714640017422], [0.3874207212216568, 0.6125792787783432], [0.5818490808403997, 0.41815091915960034], [0.2684615906116483, 0.7315384093883517], [0.5439697768358237, 0.45603022316417635], [0.5646556011012593, 0.43534439889874066], [0.6739067502877752, 0.3260932497122247], [0.4374721867673529, 0.5625278132326471], [0.4521856342175232, 0.5478143657824768], [0.13170087620358897, 0.868299123796411], [0.6767946344665222, 0.3232053655334778], [0.5007160929149557, 0.4992839070850444], [0.7774285085760781, 0.22257149142392185], [0.6519320392971242, 0.3480679607028759], [0.2546183366737041, 0.7453816633262959], [0.5755938943346637, 0.4244061056653363], [0.5201639770163562, 0.47983602298364375], [0.3626354303672459, 0.6373645696327542], [0.5948153627418323, 0.4051846372581676], [0.49801355875249875, 0.5019864412475011], [0.4072796858880742, 0.5927203141119258], [0.4915242809349924, 0.5084757190650077], [0.49976024677239883, 0.5002397532276012], [0.507689395434596, 0.49231060456540404], [0.7035142260878124, 0.29648577391218756], [0.6314825218210207, 0.3685174781789793], [0.41641095840922465, 0.5835890415907754], [0.5309336102563924, 0.4690663897436076], [0.4537463879906368, 0.5462536120093632], [0.6075712264755931, 0.3924287735244068], [0.44279369403479385, 0.5572063059652063], [0.5659374339918267, 0.4340625660081733], [0.6414387584653924, 0.3585612415346076], [0.4404114611440056, 0.5595885388559944], [0.4412564029694763, 0.5587435970305238], [0.7495091685305814, 0.2504908314694186], [0.6251307157083813, 0.37486928429161864], [0.31842611180761377, 0.6815738881923862], [0.6127138119212515, 0.38728618807874843], [0.6934710009411942, 0.30652899905880576], [0.457158698147946, 0.542841301852054], [0.42090855095887525, 0.5790914490411248], [0.48322475567307877, 0.5167752443269212], [0.416139896654872, 0.583860103345128], [0.5093329663071144, 0.49066703369288556], [0.44799360253583925, 0.5520063974641608], [0.4749820154417152, 0.5250179845582847], [0.5733999107666359, 0.4266000892333641], [0.49245152116096214, 0.5075484788390379], [0.4866227383787434, 0.5133772616212565], [0.31783344325421903, 0.6821665567457811], [0.395421621774883, 0.6045783782251171], [0.6846011063553182, 0.3153988936446817], [0.4279516061288425, 0.5720483938711575], [0.2174822624370403, 0.7825177375629597], [0.22689988019104296, 0.773100119808957], [0.9366886351699306, 0.06331136483006936], [0.477021113245092, 0.522978886754908], [0.5252606485806638, 0.47473935141933615], [0.6605023454010166, 0.33949765459898346], [0.04911079733991452, 0.9508892026600856], [0.030864432183720078, 0.96913556781628], [0.43531096727661805, 0.564689032723382], [0.47467537912696944, 0.5253246208730306], [0.5774924439432714, 0.42250755605672874], [0.5772426441661234, 0.4227573558338767], [0.6214016089879989, 0.37859839101200105], [0.4588277764410378, 0.5411722235589621], [0.47723390865744963, 0.5227660913425505], [0.5356461722165521, 0.464353827783448], [0.012384607415535204, 0.9876153925844647], [0.07221991419460728, 0.9277800858053926], [0.8548376431201851, 0.14516235687981496], [0.513848172158914, 0.486151827841086], [0.46264094149578844, 0.5373590585042116], [0.46272118865753936, 0.5372788113424606], [0.9578475821526278, 0.04215241784737224], [0.49486443986205797, 0.505135560137942], [0.4652085614254417, 0.5347914385745582], [0.3705242893878565, 0.6294757106121436], [0.8053985434237996, 0.19460145657620054], [0.34298410369319915, 0.6570158963068008], [0.5727490091804642, 0.42725099081953577], [0.4746382393637447, 0.5253617606362553], [0.4595614908120733, 0.5404385091879267], [0.6510756370936731, 0.3489243629063269], [0.8936429898857992, 0.10635701011420082], [0.398615530104307, 0.6013844698956929], [0.6608756509254942, 0.3391243490745058], [0.4588768580291964, 0.5411231419708036], [0.4743087445961976, 0.5256912554038025], [0.4291954058172974, 0.5708045941827026], [0.6386181746803211, 0.36138182531967883], [0.5930611437995343, 0.40693885620046555], [0.4351407428467675, 0.5648592571532325], [0.5713341586818061, 0.4286658413181938], [0.577676493482783, 0.42232350651721695], [0.5445653691013556, 0.45543463089864455], [0.36443868353780723, 0.6355613164621928], [0.3561864880245582, 0.6438135119754418], [0.48669238118256797, 0.513307618817432], [0.36281122260570103, 0.6371887773942989], [0.5851539552330952, 0.41484604476690473], [0.4225423941455163, 0.5774576058544837], [0.5726799532854671, 0.42732004671453305], [0.4151162693153283, 0.5848837306846718], [0.4718201717869731, 0.5281798282130269], [0.60758732914284, 0.39241267085716003], [0.2828396893612038, 0.7171603106387963], [0.12876537792923828, 0.8712346220707617], [0.5266824846491427, 0.47331751535085725], [0.6529479850066993, 0.34705201499330074], [0.5160461363504161, 0.48395386364958404], [0.4778407533060343, 0.5221592466939657], [0.4574006505561129, 0.5425993494438872], [0.5302534929565081, 0.46974650704349186], [0.8340833470889915, 0.16591665291100857], [0.6812257565939294, 0.3187742434060705], [0.4439736911888192, 0.5560263088111808], [0.6100865398817453, 0.3899134601182546], [0.5458503355820815, 0.45414966441791843], [0.5354229210845506, 0.46457707891544936], [0.8837786444968486, 0.11622135550315135], [0.5618948504525706, 0.43810514954742946], [0.4775687415899026, 0.5224312584100974], [0.6965246081528952, 0.30347539184710487], [0.432352179210234, 0.567647820789766], [0.4636012038564121, 0.5363987961435879], [0.5169459713258034, 0.48305402867419645], [0.42142619427404737, 0.5785738057259526], [0.5484401497571755, 0.4515598502428245], [0.45699743322717523, 0.5430025667728248], [0.642828498556789, 0.35717150144321097], [0.4614294102248041, 0.5385705897751958], [0.5109453311844935, 0.4890546688155066], [0.5691614604292702, 0.4308385395707299], [0.49984302339706704, 0.500156976602933], [0.5836588084813525, 0.4163411915186474], [0.5001269258681347, 0.4998730741318654], [0.05683755546258234, 0.9431624445374176], [0.5618553863083915, 0.4381446136916085], [0.31532891876964075, 0.6846710812303592], [0.4989619063068966, 0.5010380936931034], [0.493741297420796, 0.5062587025792039], [0.4580648687421711, 0.541935131257829], [0.5958116126460075, 0.4041883873539926], [0.6398340779400133, 0.3601659220599866], [0.5260069298488125, 0.4739930701511876], [0.37996707344805014, 0.6200329265519499], [0.795886529878292, 0.20411347012170797], [0.5785826561417168, 0.4214173438582832], [0.5871874795301281, 0.412812520469872], [0.22077065746685556, 0.7792293425331444], [0.345528545831334, 0.6544714541686659], [0.9853355226266929, 0.014664477373307231], [0.6215060533445681, 0.3784939466554319], [0.6098002950870309, 0.3901997049129691], [0.3742571262108959, 0.6257428737891042], [0.30134508877774635, 0.6986549112222536], [0.6886132013931592, 0.31138679860684076], [0.5333149789297246, 0.46668502107027543], [0.5212764691215772, 0.4787235308784227], [0.5532435084987696, 0.4467564915012304], [0.4922446142</t>
+          <t xml:space="preserve">[[0.018894435328766362, 0.9811055646712337], [0.07829988529436596, 0.9217001147056341], [0.7874984493876551, 0.2125015506123448], [0.4822232564627963, 0.5177767435372037], [0.7013317675942052, 0.2986682324057948], [0.9189512015865696, 0.08104879841343045], [0.2680191779571743, 0.7319808220428258], [0.386014642205631, 0.613985357794369], [0.4083812735781414, 0.5916187264218585], [0.09872476254709321, 0.9012752374529067], [0.8712531537347065, 0.1287468462652936], [0.45560230790258527, 0.5443976920974147], [0.9287864973384384, 0.07121350266156154], [0.48238021041854223, 0.5176197895814577], [0.5653093276308682, 0.43469067236913184], [0.555853813460551, 0.444146186539449], [0.38383350827505225, 0.6161664917249478], [0.5382402373921074, 0.46175976260789253], [0.45132254131499144, 0.5486774586850085], [0.0135798155443403, 0.9864201844556597], [0.6613313896046958, 0.33866861039530416], [0.6240387727395554, 0.37596122726044445], [0.300215433452904, 0.6997845665470959], [0.6268567136961216, 0.3731432863038784], [0.5544041051309884, 0.44559589486901163], [0.9058907059593639, 0.09410929404063606], [0.2557101977883714, 0.7442898022116287], [0.41688563463827544, 0.5831143653617246], [0.5775954890753108, 0.4224045109246892], [0.2908686173568286, 0.7091313826431713], [0.5957563218762967, 0.4042436781237033], [0.3919712283167271, 0.6080287716832729], [0.39974717221540834, 0.6002528277845917], [0.3274416763965481, 0.6725583236034519], [0.4880759205504328, 0.5119240794495672], [0.5017535270244227, 0.4982464729755774], [0.38852957463505333, 0.6114704253649468], [0.20199069310341203, 0.798009306896588], [0.3395279302044918, 0.6604720697955082], [0.10423493089940472, 0.8957650691005953], [0.743132526683856, 0.25686747331614407], [0.8807558143306523, 0.11924418566934779], [0.234874119031065, 0.7651258809689351], [0.43830470503168834, 0.5616952949683116], [0.2324743220092986, 0.7675256779907014], [0.575828187177433, 0.4241718128225671], [0.6922828972320009, 0.30771710276799913], [0.8218269039388079, 0.178173096061192], [0.3730906306212801, 0.6269093693787199], [0.524642068949804, 0.47535793105019597], [0.39281462804884393, 0.6071853719511562], [0.43213408670855863, 0.5678659132914414], [0.31384983030652175, 0.6861501696934783], [0.8572718486257315, 0.14272815137426845], [0.10118686540092375, 0.8988131345990762], [0.6319331495573577, 0.36806685044264226], [0.6935890392899383, 0.30641096071006174], [0.49076897318455454, 0.5092310268154454], [0.5749121008886754, 0.42508789911132455], [0.5633091041443525, 0.43669089585564747], [0.33442488088203987, 0.6655751191179601], [0.02750288260795796, 0.9724971173920421], [0.9800023054840624, 0.019997694515937556], [0.38434669020178996, 0.61565330979821], [0.7002537187378739, 0.29974628126212605], [0.17087173887197593, 0.8291282611280241], [0.41451891767824744, 0.5854810823217526], [0.4505480708236977, 0.5494519291763024], [0.6898833990900016, 0.3101166009099983], [0.5215647126253365, 0.47843528737466356], [0.2552826796080802, 0.7447173203919197], [0.44879077477211365, 0.5512092252278863], [0.8381319366155018, 0.16186806338449825], [0.9069779766325543, 0.09302202336744567], [0.5919177843054524, 0.40808221569454756], [0.8929607218328721, 0.10703927816712785], [0.36215423567494204, 0.6378457643250579], [0.08312365779052264, 0.9168763422094773], [0.19259335867776894, 0.807406641322231], [0.3507876036133295, 0.6492123963866704], [0.9386280459738758, 0.06137195402612409], [0.420571996420012, 0.5794280035799881], [0.589130347077993, 0.4108696529220069], [0.3178318363312822, 0.6821681636687178], [0.8313642425175771, 0.16863575748242288], [0.4864186393650648, 0.5135813606349352], [0.4563356831822423, 0.5436643168177577], [0.5326412747197192, 0.46735872528028083], [0.3739745056964492, 0.6260254943035509], [0.14916382851769694, 0.8508361714823031], [0.4385054828075477, 0.5614945171924522], [0.26037394093082916, 0.7396260590691709], [0.12934864378651548, 0.8706513562134846], [0.32143060637317794, 0.678569393626822], [0.9490362466079217, 0.0509637533920783], [0.5238394081435165, 0.4761605918564836], [0.8576051692121378, 0.1423948307878622], [0.34518467138114495, 0.654815328618855], [0.08772455956969234, 0.9122754404303076], [0.5392317662782143, 0.46076823372178566], [0.5941124005026205, 0.40588759949737946], [0.6206891886639945, 0.37931081133600547], [0.1713664615114123, 0.8286335384885878], [0.5735116155918816, 0.42648838440811837], [0.5188114390288995, 0.4811885609711005], [0.3687296324372023, 0.6312703675627978], [0.588608005171679, 0.411391994828321], [0.557537767159363, 0.442462232840637], [0.7497888517399728, 0.25021114826002716], [0.5187750459812231, 0.4812249540187768], [0.44191017162011337, 0.5580898283798865], [0.7724075489610488, 0.22759245103895118], [0.49360696304574836, 0.5063930369542516], [0.35763640244424355, 0.6423635975557566], [0.18930524130105628, 0.8106947586989437], [0.5207319557750709, 0.47926804422492897], [0.6275692888419494, 0.37243071115805065], [0.31213685940054636, 0.6878631405994536], [0.5863717310125741, 0.4136282689874258], [0.33523906095461425, 0.6647609390453858], [0.2591031046482083, 0.7408968953517917], [0.461866443714615, 0.5381335562853851], [0.8160954189769403, 0.18390458102305984], [0.03734921725935444, 0.9626507827406455], [0.4660580971609561, 0.5339419028390439], [0.9608399278887978, 0.03916007211120212], [0.8260315891014951, 0.173968410898505], [0.22393498910439588, 0.7760650108956041], [0.2902249561128362, 0.7097750438871637], [0.27629709515501405, 0.7237029048449859], [0.5997024733924627, 0.40029752660753715], [0.9618223075585013, 0.03817769244149875], [0.6814153376140399, 0.31858466238596006], [0.6429434278466708, 0.3570565721533293], [0.6901857481158695, 0.3098142518841305], [0.5687701471261184, 0.43122985287388166], [0.14497379287227727, 0.8550262071277228], [0.6040999643644055, 0.39590003563559445], [0.7634441666952911, 0.23655583330470883], [0.18946741696828842, 0.8105325830317115], [0.3147990118259964, 0.6852009881740035], [0.20354620015660793, 0.796453799843392], [0.4856394023472292, 0.5143605976527709], [0.9730300517027232, 0.026969948297276853], [0.7955153965825391, 0.20448460341746091], [0.7551797070852301, 0.24482029291476992], [0.18104679465141063, 0.8189532053485894], [0.6918710640044076, 0.30812893599559243], [0.5454911944556091, 0.4545088055443908], [0.6923608330796153, 0.3076391669203848], [0.32316341112303654, 0.6768365888769635], [0.10265394300698305, 0.8973460569930171], [0.6939836476957827, 0.3060163523042173], [0.2463745144195035, 0.7536254855804965], [0.5829947666696456, 0.4170052333303544], [0.15893707978328767, 0.8410629202167124], [0.16926081768125267, 0.8307391823187474], [0.7483368873457356, 0.2516631126542644], [0.6308797616506188, 0.3691202383493813], [0.3483655665882605, 0.6516344334117395], [0.06962248905190799, 0.930377510948092], [0.2340292539200973, 0.7659707460799028], [0.8129719817696083, 0.18702801823039178], [0.5132030505089015, 0.4867969494910986], [0.8218087360101605, 0.17819126398983942], [0.18745482186076776, 0.8125451781392323], [0.5098309419808954, 0.4901690580191046], [0.73694320166644, 0.26305679833356005], [0.3225490454914482, 0.6774509545085519], [0.3235826018038548, 0.6764173981961452], [0.3170069135685502, 0.6829930864314497], [0.618832805947002, 0.3811671940529981], [0.5052129162466017, 0.49478708375339836], [0.604238712888215, 0.39576128711178504], [0.6869951181769938, 0.31300488182300623], [0.7934963025096126, 0.20650369749038738], [0.38350342713204544, 0.6164965728679546], [0.7347240490292721, 0.2652759509707279], [0.7269413776913584, 0.27305862230864164], [0.24600296767402924, 0.7539970323259707], [0.41000079034654385, 0.5899992096534562], [0.9319915867045667, 0.06800841329543329], [0.6561206022311934, 0.34387939776880666], [0.2241233724302897, 0.7758766275697102], [0.5897629496199058, 0.4102370503800942], [0.002080157254594823, 0.9979198427454052], [0.4263292722650803, 0.5736707277349197], [0.3396835898400599, 0.6603164101599401], [0.8224848190157044, 0.1775151809842956], [0.913743545167787, 0.08625645483221303], [0.8855472983222274, 0.11445270167777254], [0.7550842097516869, 0.24491579024831314], [0.5189427840449741, 0.481057215955026], [0.9574829301182542, 0.042517069881745854], [0.988086533085509, 0.011913466914490972], [0.3500370549870238, 0.6499629450129762], [0.3693520502093396, 0.6306479497906604], [0.3826104612014985, 0.6173895387985016], [0.6642672092784853, 0.3357327907215148], [0.15300900844340506, 0.8469909915565949], [0.7437177776606884, 0.2562822223393117], [0.9812736281563953, 0.018726371843604678], [0.703197983664748, 0.296802016335252], [0.3646340966346805, 0.6353659033653195], [0.354079535743981, 0.645920464256019], [0.03174349978704193, 0.9682565002129581], [0.584478006226831, 0.41552199377316895], [0.2258864850974693, 0.7741135149025306], [0.49459551557758163, 0.5054044844224184], [0.5785657461416056, 0.4214342538583945], [0.39986723493538434, 0.6001327650646158], [0.5244355454569842, 0.47556445454301577], [0.3973778997739894, 0.6026221002260106], [0.6129680310513619, 0.38703196894863806], [0.05797606383384912, 0.9420239361661508], [0.4810119855132733, 0.5189880144867267], [0.7571184161784031, 0.24288158382159689], [0.7795165718561541, 0.22048342814384597], [0.06210368394987927, 0.9378963160501207], [0.4285094064637592, 0.5714905935362408], [0.37981112162184266, 0.6201888783781574], [0.6128949503716525, 0.38710504962834735], [0.7439299007027085, 0.2560700992972915], [0.4096363658483466, 0.5903636341516534], [0.3645085584219807, 0.6354914415780193], [0.6330516320366796, 0.36694836796332037], [0.5047402743016779, 0.49525972569832216], [0.446776577629607, 0.5532234223703931], [0.973367851365145, 0.026632148634854944], [0.6068818440785074, 0.3931181559214926], [0.6370074135193954, 0.3629925864806046], [0.29982887771816497, 0.7001711222818351], [0.5465446393757063, 0.45345536062429365], [0.7636538934040897, 0.23634610659591032], [0.5558245027060228, 0.44417549729397715], [0.884079937952384, 0.11592006204761597], [0.16873832231315797, 0.8312616776868421], [0.37022853372725995, 0.62977146627274], [0.8792981473668928, 0.12070185263310707], [0.5829029024953443, 0.41709709750465584], [0.05756455841615733, 0.9424354415838426], [0.07296716220797153, 0.9270328377920285], [0.43839051770981896, 0.561609482290181], [0.6412925922637011, 0.35870740773629894], [0.9387510415151119, 0.06124895848488818], [0.39937125901094495, 0.600628740989055], [0.6860037080250233, 0.31399629197497675], [0.8348200415000977, 0.1651799584999023], [0.20916796165948892, 0.7908320383405112], [0.5352873983126972, 0.46471260168730266], [0.41205588870593274, 0.5879441112940673], [0.6323475535077191, 0.367652446492281], [0.1578000147320749, 0.8421999852679252], [0.7173783577351034, 0.28262164226489667], [0.40771737197081487, 0.5922826280291851], [0.39288169296506925, 0.6071183070349307], [0.6138887017138496, 0.3861112982861504], [0.35339802526429365, 0.6466019747357064], [0.9309958732254479, 0.06900412677455209], [0.9160673502805317, 0.08393264971946836], [0.9598677197658861, 0.04013228023411381], [0.6480279671393694, 0.3519720328606307], [0.5171957981565294, 0.4828042018434706], [0.639083757436837, 0.360916242563163], [0.149909797096894, 0.850090202903106], [0.36147907045847727, 0.6385209295415227], [0.7315754348023982, 0.2684245651976019], [0.5484304440643897, 0.45156955593561043], [0.46699584556713986, 0.5330041544328602], [0.17606241119955465, 0.8239375888004453], [0.7007810495839386, 0.2992189504160614], [0.4900754690850443, 0.5099245309149557], [0.59589241718639, 0.40410758281361003], [0.2917975444293028, 0.7082024555706973], [0.005599404783639264, 0.9944005952163608], [0.7236693135309717, 0.27633068646902836], [0.6512876691242062, 0.34871233087579384], [0.8059081483714291, 0.19409185162857093], [0.4314597290157449, 0.568540270984255], [0.5670133341060344, 0.4329866658939656], [0.6849231434861888, 0.3150768565138113], [0.3766532514976175, 0.6233467485023826], [0.4161877660372877, 0.5838122339627122], [0.5707521412950559, 0.42924785870494403], [0.8350723831532031, 0.1649276168467969], [0.6694507641603311, 0.33054923583966894], [0.018460403929513255, 0.9815395960704867], [0.9651031305664274, 0.03489686943357272], [0.5545568062975672, 0.44544319370243285], [0.8329564966429737, 0.16704350335702625], [0.3987852005435801, 0.6012147994564199], [0.2559691102029646, 0.7440308897970354], [0.6009401826190833, 0.3990598173809168], [0.6663899154918907, 0.33361008450810925], [0.5534478836014997, 0.44655211639850045], [0.8487300669565689, 0.15126993304343114], [0.6637087692625353, 0.33629123073746475], [0.7880922021235478, 0.21190779787645228], [0.7746239507628757, 0.22537604923712437], [0.6101927312953906, 0.3898072687046094], [0.48780691184858854, 0.5121930881514115], [0.5897519871462066, 0.41024801285379336], [0.5920442674561592, 0.4079557325438407], [0.2742389535416993, 0.7257610464583006], [0.5779432557382386, 0.42205674426176143], [0.903117536822707, 0.09688246317729292], [0.302569913084809, 0.697430086915191], [0.9885720116433463, 0.01142798835665364], [0.1997351862095566, 0.8002648137904435], [0.3083730768814891, 0.6916269231185109], [0.7268978942015825, 0.2731021057984175], [0.04367977610731978, 0.9563202238926803], [0.29461688360011334, 0.7053831163998866], [0.5521139859503954, 0.44788601404960454], [0.5855739007453664, 0.41442609925463353], [0.34992008689572873, 0.6500799131042712], [0.6972461428262862, 0.30275385717371395], [0.2941954302739168, 0.7058045697260831], [0.757590728837251, 0.24240927116274907], [0.10312299256849784, 0.8968770074315021], [0.5109551928930689, 0.4890448071069311], [0.21120412922696705, 0.7887958707730329], [0.6086138532461722, 0.39138614675382777], [0.7859244910052382, 0.21407550899476185], [0.47021075706297044, 0.5297892429370296], [0.4814895746642054, 0.5185104253357947], [0.8046047281900193, 0.19539527180998081], [0.6008230691045694, 0.39917693089543066], [0.3223345543397386, 0.6776654456602614], [0.8689616561814301, 0.13103834381856996], [0.63227555961694, 0.36772444038305996], [0.11202326038982355, 0.8879767396101765], [0.281063653076328, 0.7189363469236719], [0.6210765943231379, 0.378923405676862], [0.21679113853177112, 0.7832088614682289], [0.9806204319557718, 0.01937956804422818], [0.20825523208169947, 0.7917447679183005], [0.027284463136929917, 0.97271553686307], [0.08772058417400844, 0.9122794158259916], [0.7312734333790497, 0.2687265666209503], [0.01860393439522907, 0.981396065604771], [0.3281323219557193, 0.6718676780442807], [0.729872729038616, 0.2701272709613839], [0.42264551064590344, 0.5773544893540965], [0.013937675566105928, 0.986062324433894], [0.15863042212280715, 0.8413695778771929], [0.6121136552149755, 0.3878863447850245], [0.6400741997983249, 0.3599258002016751], [0.1799655574127945, 0.8200344425872056], [0.023497894933422477, 0.9765021050665775], [0.37061827914545264, 0.6293817208545474], [0.18349259356982256, 0.8165074064301774], [0.3679839872914847, 0.6320160127085153], [0.2510304959484499, 0.74896950405155], [0.5091689165520796, 0.4908310834479204], [0.4414057674020629, 0.5585942325979372], [0.6015400318742512, 0.39845996812574885], [0.5296791125348256, 0.4703208874651744], [0.6644653746522402, 0.3355346253477598], [0.6333216989599388, 0.3666783010400611], [0.1120643144169863, 0.8879356855830136], [0.9856523801726785, 0.014347619827321354], [0.44998658167520195, 0.550013418324798], [0.8042170613994559, 0.19578293860054405], [0.4598863314119257, 0.5401136685880743], [0.2889579698680364, 0.7110420301319635], [0.36630848926795906, 0.633691510732041], [0.9097075880453857, 0.09029241195461438], [0.4139989177617613, 0.5860010822382387], [0.1479535052813747, 0.8520464947186253], [0.5733786442982245, 0.42662135570177556], [0.5063261691837025, 0.49367383081629745], [0.5877783395719934, 0.41222166042800656], [0.4972046896159273, 0.5027953103840728], [0.27157933652740773, 0.7284206634725923], [0.4735420483743138, 0.5264579516256862], [0.49936914049314673, 0.5006308595068533], [0.30697369946097985, 0.6930263005390203], [0.3862419587162, 0.6137580412838001], [0.05863358814221657, 0.9413664118577835], [0.03643780936355583, 0.9635621906364441], [0.6729372933325648, 0.3270627066674352], [0.3582965806858408, 0.6417034193141593], [0.3804451657720428, 0.6195548342279573], [0.1890711593915232, 0.8109288406084769], [0.5106383627810743, 0.48936163721892567], [0.6069865715846362, 0.3930134284153638], [0.7144035195450984, 0.28559648045490166], [0.45822500188216414, 0.5417749981178359], [0.5370441833852484, 0.46295581661475155], [0.5789019797631084, 0.4210980202368916], [0.9686472635214383, 0.031352736478561655], [0.12464047840514814, 0.8753595215948519], [0.20275583719114895, 0.797244162808851], [0.6201168774710285, 0.3798831225289715], [0.4408056778697104, 0.5591943221302896], [0.2872014651644661, 0.712798534835534], [0.6973695011424461, 0.302630498857554], [0.569032504403764, 0.4309674955962361], [0.552441813341504, 0.4475581866584961], [0.1495054132327422, 0.8504945867672579], [0.6772795453974791, 0.3227204546025209], [0.9125839528622974, 0.08741604713770255], [0.8197831042361186, 0.18021689576388142], [0.9919313890264163, 0.008068610973583693], [0.08113807249413744, 0.9188619275058627], [0.3478810552185661, 0.6521189447814338], [0.41366484504732415, 0.5863351549526759], [0.5954384545382128, 0.40456154546178735], [0.6420406455233392, 0.35795935447666094], [0.26881735635938686, 0.7311826436406133], [0.601564532667428, 0.39843546733257196], [0.5707030315001089, 0.429296968499891], [0.6477446308014215, 0.3522553691985786], [0.4210720274979409, 0.5789279725020591], [0.4188205438559192, 0.5811794561440807], [0.42877912177150607, 0.5712208782284939], [0.9282347756771937, 0.07176522432280626], [0.6928349595369176, 0.3071650404630824], [0.6121117077688456, 0.38788829223115445], [0.9152064247266087, 0.08479357527339124], [0.5148711294200906, 0.48512887057990933], [0.2331903351394754, 0.7668096648605246], [0.8458455676073234, 0.15415443239267648], [0.4124981999226273, 0.5875018000773727], [0.43711981430333224, 0.5628801856966678], [0.44039032359045593, 0.5596096764095441], [0.7379738471761618, 0.2620261528238383], [0.2994749327010996, 0.7005250672989003], [0.43478290058205316, 0.5652170994179468], [0.734603268160068, 0.2653967318399319], [0.3961987590990316, 0.6038012409009683], [0.700666384021975, 0.2993336159780251], [0.4148565781123556, 0.5851434218876445], [0.934086655127546, 0.06591334487245407], [0.7945578807997791, 0.2054421192002208], [0.3201018521920866, 0.6798981478079134], [0.8761764527498813, 0.12382354725011874], [0.5572987983557158, 0.4427012016442841], [0.8442608812685883, 0.15573911873141155], [0.5459383981182115, 0.45406160188178846], [0.39846557910275876, 0.6015344208972412], [0.4624980485016379, 0.5375019514983621], [0.6119255820847089, 0.3880744179152911], [0.11064318321012287, 0.889356816789877], [0.5886352616904708, 0.4113647383095293], [0.40998510213314565, 0.5900148978668543], [0.34122231759097316, 0.6587776824090269], [0.0842666574864416, 0.9157333425135584], [0.9208779076674612, 0.0791220923325387], [0.7280681660925432, 0.27193183390745684], [0.5046297830273146, 0.49537021697268535], [0.7562123367120287, 0.24378766328797138], [0.5109910127130852, 0.4890089872869147], [0.6153385531255797, 0.38466144687442017], [0.5297400457828092, 0.4702599542171908], [0.5506421117783424, 0.4493578882216576], [0.2056937214682866, 0.7943062785317134], [0.5930260734063023, 0.4069739265936977], [0.32697954928012757, 0.6730204507198724], [0.348314099821901, 0.651685900178099], [0.3721492775573747, 0.6278507224426252], [0.1674202286330696, 0.8325797713669305], [0.28350047155893504, 0.7164995284410649], [0.9349885698960221, 0.065011430103978], [0.7722291303872426, 0.22777086961275736], [0.63872610222131, 0.3612738977786901], [0.9987812405028198, 0.0012187594971801734], [0.4604032233504369, 0.5395967766495632], [0.897101882445433, 0.10289811755456693], [0.5011950340597069, 0.4988049659402932], [0.47691089639995005, 0.52308910360005], [0.34583948857458674, 0.6541605114254133], [0.09023791018185416, 0.9097620898181459], [0.25493502138083957, 0.7450649786191603], [0.4340506196263831, 0.5659493803736169], [0.9966726429631017, 0.003327357036898438], [0.2734679070053389, 0.726532092994661], [0.25541947252886105, 0.744580527471139], [0.3096318054441722, 0.6903681945558278], [0.275955263409985, 0.724044736590015], [0.6617794008709761, 0.3382205991290239], [0.5796097785503966, 0.42039022144960336], [0.8992596827750952, 0.10074031722490485], [0.8253969693867423, 0.17460303061325777], [0.6212678932821932, 0.3787321067178068], [0.33772101085343853, 0.6622789891465615], [0.7186687651872844, 0.2813312348127156], [0.30630618337885523, 0.6936938166211447], [0.3531990415900139, 0.6468009584099862], [0.3077882753503415, 0.6922117246496585], [0.3344531982981163, 0.6655468017018836], [0.49950214328446213, 0.5004978567155378], [0.4940269864044441, 0.5059730135955559], [0.8547362758681328, 0.14526372413186722], [0.49640928827352965, 0.5035907117264703], [0.6593131674520532, 0.34068683254794685], [0.20550153308700503, 0.794498466912995], [0.350527701316947, 0.649472298683053], [0.9472649339293889, 0.05273506607061096], [0.8360644722730709, 0.16393552772692904], [0.4799122535188563, 0.5200877464811436], [0.6332779985600696, 0.36672200143993045], [0.35736433303742154, 0.6426356669625786], [0.4976334166744111, 0.502366583325589], [0.7015906149629328, 0.29840938503706704], [0.7355726356179938, 0.2644273643820062], [0.5128601814290388, 0.4871398185709613], [0.16028740100297814, 0.8397125989970218], [0.9278798661460047, 0.07212013385399531], [0.11619503153801278, 0.8838049684619873], [0.2027426452070913, 0.7972573547929087], [0.6311052096061218, 0.36889479039387807], [0.0492956919540311, 0.9507043080459688], [0.2993756871705171, 0.7006243128294828], [0.27554399393915685, 0.7244560060608431], [0.2827342090385561, 0.7172657909614438], [0.7690790812714144, 0.23092091872858556], [0.7709904843462831, 0.22900951565371688], [0.7622441151371484, 0.23775588486285157], [0.4460017592208716, 0.5539982407791284], [0.6332619972446835, 0.3667380027553166], [0.4765802854547569, 0.523419714545243], [0.57413035162299, 0.42586964837701], [0.3687155175126233, 0.6312844824873767], [0.6748814797356132, 0.3251185202643868], [0.9104022455482839, 0.08959775445171622], [0.9497268025403365, 0.05027319745966356], [0.027353935652812765, 0.9726460643471871], [0.5433113829225059, 0.4566886170774941], [0.30331399825268374, 0.6966860017473162], [0.035697638738524856, 0.9643023612614751], [0.6314721643512784, 0.3685278356487216], [0.5479347584045144, 0.45206524159548556], [0.4838928603833442, 0.5161071396166558], [0.37942883812368244, 0.6205711618763177], [0.20608224258359853, 0.7939177574164016], [0.1720967662153275, 0.8279032337846726], [0.2571146278677973, 0.7428853721322026], [0.6892812309485463, 0.31071876905145374], [0.28862695068010236, 0.7113730493198976], [0.12824704868448708, 0.8717529513155129], [0.34173250069392735, 0.6582674993060726], [0.5794446808660336, 0.4205553191339663], [0.5943638100953252, 0.40563618990467476], [0.5870863850831677, 0.41291361491683237], [0.37295791102284176, 0.6270420889771582], [0.5935247913164249, 0.4064752086835751], [0.9234362546644118, 0.07656374533558825], [0.4858507295183371, 0.5141492704816629], [0.8370881528870979, 0.16291184711290208], [0.7794220745306758, 0.2205779254693241], [0.4905351618552385, 0.5094648381447615], [0.3476976715153848, 0.6523023284846153], [0.3610430556262979, 0.6389569443737022], [0.6604740551460296, 0.3395259448539703], [0.4354020582789674, 0.5645979417210326], [0.07041056794350913, 0.9295894320564909], [0.7928807434065632, 0.2071192565934369], [0.19887310804760794, 0.8011268919523921], [0.017577684780949263, 0.9824223152190508], [0.8330554128347674, 0.1669445871652326], [0.5805901394377243, 0.4194098605622758], [0.22677665143389852, 0.7732233485661014], [0.4830829177962169, 0.5169170822037831], [0.9022565637219209, 0.09774343627807922], [0.7395693943072361, 0.26043060569276383], [0.5473805126320378, 0.45261948736796215], [0.17709404433142026, 0.8229059556685798], [0.6079699630567706, 0.39203003694322935], [0.6820623775514908, 0.3179376224485091], [0.26155215410562527, 0.7384478458943746], [0.7101253955392209, 0.28987460446077906], [0.43078727133847267, 0.5692127286615274], [0.40834868005320496, 0.5916513199467951], [0.3887964014748491, 0.6112035985251509], [0.626087710792767, 0.37391228920723285], [0.0010414678615704373, 0.9989585321384294], [0.29192999555675925, 0.7080700044432406], [0.5396895258621882, 0.4603104741378119], [0.9981207327335985, 0.0018792672664015924], [0.675049377706448, 0.324950622293552], [0.043940136812013204, 0.9560598631879867], [0.42642922443944536, 0.5735707755605547], [0.1926746373029361, 0.8073253626970639], [0.29168199262904015, 0.7083180073709598], [0.10998142956388991, 0.8900185704361101], [0.7850997508474736, 0.2149002491525263], [0.9678475784326103, 0.03215242156738967], [0.05384060275603049, 0.9461593972439695], [0.7921014698099317, 0.20789853019006826], [0.5300628133552414, 0.46993718664475864], [0.14806026811197895, 0.8519397318880211], [0.31996524655603187, 0.6800347534439681], [0.6108866267101128, 0.3891133732898872], [0.5702532054000875, 0.4297467945999125], [0.22803777606573572, 0.7719622239342643], [0.6713274309127917, 0.3286725690872083], [0.3931602151917351, 0.606839784808265], [0.7382086014081757, 0.26179139859182426], [0.5190688122917135, 0.4809311877082864], [0.24509590989384744, 0.7549040901061526], [0.6008430383419969, 0.39915696165800313], [0.9640219499170918, 0.03597805008290817], [0.23309533323829665, 0.7669046667617033], [0.31813117324933704, 0.6818688267506631], [0.6529896684506866, 0.3470103315493134], [0.5289707161391222, 0.4710292838608779], [0.3956667000161108, 0.6043332999838892], [0.770861933254124, 0.22913806674587608], [0.8686564483359845, 0.1313435516640154], [0.7031897455967682, 0.29681025440323183], [0.582798903034651, 0.41720109696534907], [0.2153794768552531, 0.784620523144747], [0.7339646081485215, 0.26603539185147856], [0.1731097998880956, 0.8268902001119045], [0.6605990278173373, 0.33940097218266263], [0.6529923760252413, 0.34700762397475876], [0.5843009345831761, 0.41569906541682383], [0.001330746929666284, 0.9986692530703338], [0.48461663085204226, 0.5153833691479577], [0.906222041545405, 0.09377795845459508], [0.4844162830832402, 0.5155837169167597], [0.35844634139185594, 0.6415536586081441], [0.9978619096126088, 0.0021380903873912714], [0.2963729250606114, 0.7036270749393886], [0.6012792512202171, 0.398720748779783], [0.2557101977883714, 0.7442898022116287], [0.528355120703202, 0.471644879296798], [0.6209726457662162, 0.3790273542337838], [0.5519961764799749, 0.44800382352002505], [0.900327598722857, 0.09967240127714294], [0.23953182973397744, 0.7604681702660226], [0.9241586711114491, 0.0758413288885509], [0.05349722428713043, 0.9465027757128696], [0.16344849539486112, 0.8365515046051388], [0.6173882702349704, 0.38261172976502955], [0.6101391428896062, 0.3898608571103938], [0.09132067876568122, 0.9086793212343188], [0.442010353728938, 0.5579896462710621], [0.5611478620009247, 0.43885213799907535], [0.3568433841117901, 0.6431566158882098], [0.9629632794334338, 0.037036720566566185], [0.7276156932666609, 0.27238430673333913], [0.45442029025464287, 0.5455797097453572], [0.19614944979526938, 0.8038505502047306], [0.4641739086795168, 0.5358260913204832], [0.6073241546616697, 0.3926758453383303], [0.7320376880482993, 0.2679623119517007], [0.9636638838373631, 0.03633611616263676], [0.4865369942409494, 0.5134630057590506], [0.5105953149484425, 0.4894046850515575], [0.5620091917931803, 0.4379908082068197], [0.33692848529478714, 0.6630715147052129], [0.5007327343555488, 0.4992672656444513], [0.19142807770522424, 0.8085719222947758], [0.49849348808685556, 0.5015065119131444], [0.46725142145929405, 0.5327485785407059], [0.4863299628354678, 0.5136700371645323], [0.5275774992068528, 0.4724225007931472], [0.6352754727107334, 0.3647245272892667], [0.5409260776109692, 0.4590739223890308], [0.8118117157050396, 0.18818828429496048], [0.6672496134655587, 0.33275038653444144], [0.27299549206652324, 0.7270045079334768], [0.879468638467241, 0.12053136153275901], [0.3077511845922306, 0.6922488154077694], [0.720113324612971, 0.279886675387029], [0.7242801832088597, 0.2757198167911403], [0.2346904594590252, 0.7653095405409749], [0.4389761122548118, 0.5610238877451883], [0.3843316434407138, 0.6156683565592862], [0.23669244122720132, 0.7633075587727987], [0.5998258802887912, 0.40017411971120864], [0.5207740085474005, 0.4792259914525995], [0.47066136462481434, 0.5293386353751857], [0.31911963449518654, 0.6808803655048135], [0.3306809486172984, 0.6693190513827016], [0.7916183095261989, 0.20838169047380112], [0.5665159210284085, 0.43348407897159147], [0.2978751528025781, 0.7021248471974219], [0.262257785108355, 0.737742214891645], [0.32850431427292176, 0.6714956857270782], [0.7449913892900538, 0.2550086107099461], [0.3026168424229953, 0.6973831575770046], [0.7347574448257187, 0.2652425551742813], [0.23442453139429886, 0.7655754686057011], [0.8857684144400313, 0.11423158555996873], [0.24698284603231596, 0.7530171539676841], [0.1798388735118535, 0.8201611264881464], [0.8130496162860974, 0.18695038371390255], [0.33908043320818143, 0.6609195667918185], [0.5787367140786625, 0.4212632859213375], [0.2774037780696147, 0.7225962219303853], [0.7391981714492896, 0.2608018285507105], [0.47675151596698173, 0.5232484840330183], [0.557221038845748, 0.442778961154252], [0.580652594551641, 0.4193474054483591], [0.1707104430943723, 0.8292895569056277], [0.7082688897375945, 0.29173111026240545], [0.5093611908243606, 0.4906388091756394], [0.3117070509760585, 0.6882929490239414], [0.12799720705841228, 0.8720027929415878], [0.4254324280084024, 0.5745675719915977], [0.7651354615911137, 0.2348645384088863], [0.5884437869511535, 0.41155621304884643], [0.7281300496866803, 0.2718699503133197], [0.02130194936238872, 0.9786980506376114], [0.7398546665757118, 0.26014533342428836], [0.7670348976171776, 0.23296510238282248], [0.3911083889988679, 0.6088916110011321], [0.09035179944566897, 0.909648200554331], [0.5558547248853976, 0.44414527511460244], [0.45872652666088326, 0.5412734733391168], [0.6022832057919579, 0.39771679420804207], [0.43608023232484644, 0.5639197676751536], [0.5783479694789375, 0.42165203052106254], [0.48736772570517606, 0.5126322742948238], [0.08581932652523915, 0.914180673474761], [0.9361856895551565, 0.06381431044484359], [0.4924818445464925, 0.5075181554535075], [0.37777850902661053, 0.6222214909733895], [0.6969389535629988, 0.3030610464370012], [0.26902158054480857, 0.7309784194551914], [0.7826361394737285, 0.2173638605262716], [0.6286024471379903, 0.3713975528620097], [0.35633095465831544, 0.6436690453416846], [0.23845149765066515, 0.7615485023493348], [0.6509659322259318, 0.34903406777406815], [0.8076522804802604, 0.19234771951973964], [0.055445350770108606, 0.9445546492298915], [0.47925169812324553, 0.5207483018767545], [0.5568449940062103, 0.4431550059937897], [0.7628687482383881, 0.23713125176161193], [0.6205085954857403, 0.37949140451425956], [0.6692436229084114, 0.3307563770915886], [0.5805633142205544, 0.41943668577944554], [0.6601150149654503, 0.33988498503454967], [0.6144433539021731, 0.3855566460978269], [0.12934020903336793, 0.8706597909666322], [0.363460510464878, 0.636539489535122], [0.541954184820517, 0.4580458151794829], [0.578567741936872, 0.42143225806312795], [0.3195151365985276, 0.6804848634014724], [0.10671223117360429, 0.8932877688263957], [0.5858423770454415, 0.4141576229545585], [0.35397291947112813, 0.6460270805288719], [0.5709137287250803, 0.4290862712749197], [0.6152803782728016, 0.38471962172719837], [0.5609567012611487, 0.43904329873885134], [0.03638067554241332, 0.9636193244575867], [0.2592549040676189, 0.740745095932381], [0.3147273701527345, 0.6852726298472654], [0.9143306128205693, 0.08566938717943064], [0.979260915683701, 0.020739084316299033], [0.3717246073753941, 0.6282753926246059], [0.6512310623888656, 0.34876893761113437], [0.6231722402392533, 0.37682775976074667], [0.4968529964433112, 0.5031470035566887], [0.9097697717103816, 0.0902302282896184], [0.7265644478619051, 0.27343555213809484], [0.8603498519319899, 0.13965014806801018], [0.3642987060893619, 0.6357012939106381], [0.5760398455791599, 0.4239601544208401], [0.44020496211113175, 0.5597950378888682], [0.6617311483901765, 0.3382688516098234], [0.7974815674554182, 0.20251843254458177], [0.7840087373219775, 0.2159912626780224], [0.17520870774876465, 0.8247912922512354], [0.4706990893086985, 0.5293009106913015], [0.18914485431178227, 0.8108551456882177], [0.5340504385631274, 0.46594956143687255], </t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">[0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 1, 1, 0, 0, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 0, 0, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 1, 1, 0, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 1, 1, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 1, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 1, 0, 1, 1, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 0, 0, 1, 0, 0, 0, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 1, 1, 0, 1, 1, 0, 0, 1, 1, 0, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 1, 0, 0, 1, 1, 0, 1, 1, 0, 0, 0, 0, 1, 0, 0, 1, 0, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 0, 1, 0, 1, 0, 0, 1, 1, 0, 1, 1, 0, 1, 0, 1, 0, 0, 0, 0, 1, </t>
+          <t>[1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 1.0, 0.0, 1.0, 1.0, 0.0, 0.0, 1.0, 1.0, 1.0, 1</t>
         </is>
       </c>
     </row>

</xml_diff>